<commit_message>
version final sin errores
</commit_message>
<xml_diff>
--- a/CodeSystem-CSCodigoDNI.xlsx
+++ b/CodeSystem-CSCodigoDNI.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.4.0</t>
+    <t>0.7.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -75,187 +75,184 @@
     <t>No display for ContactDetail</t>
   </si>
   <si>
-    <t>Jurisdiction</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Códigos para los DNI de países de America Latina y el Caribe según indicaciones de VS HL7 de V3</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Copyright</t>
+  </si>
+  <si>
+    <t>Case Sensitive</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Value Set (all codes)</t>
+  </si>
+  <si>
+    <t>Hierarchy</t>
+  </si>
+  <si>
+    <t>Compositional</t>
+  </si>
+  <si>
+    <t>Version Needed?</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>Supplements</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>NNBLZ</t>
+  </si>
+  <si>
+    <t>Belice</t>
+  </si>
+  <si>
+    <t>NNCRI</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>NNSLV</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>NNGTM</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>NNHND</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>NNMEX</t>
+  </si>
+  <si>
+    <t>México</t>
+  </si>
+  <si>
+    <t>NNNIC</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>NNPAN</t>
+  </si>
+  <si>
+    <t>Panamá</t>
+  </si>
+  <si>
+    <t>NNARG</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>NNBOL</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>NNBRA</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>NNCOL</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>NNECU</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>NNGUY</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>NNPRY</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>NNPER</t>
+  </si>
+  <si>
+    <t>Perú</t>
+  </si>
+  <si>
+    <t>NNSUR</t>
+  </si>
+  <si>
+    <t>Surinam</t>
+  </si>
+  <si>
+    <t>NNURY</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>NNVEN</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>NNCHL</t>
   </si>
   <si>
     <t>Chile</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Códigos para los DNI de países de America Latina y el Caribe según indicaciones de VS HL7 de V3</t>
-  </si>
-  <si>
-    <t>Purpose</t>
-  </si>
-  <si>
-    <t>Copyright</t>
-  </si>
-  <si>
-    <t>Case Sensitive</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>Value Set (all codes)</t>
-  </si>
-  <si>
-    <t>Hierarchy</t>
-  </si>
-  <si>
-    <t>Compositional</t>
-  </si>
-  <si>
-    <t>Version Needed?</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>complete</t>
-  </si>
-  <si>
-    <t>Supplements</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Display</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>NNBLZ</t>
-  </si>
-  <si>
-    <t>Belice</t>
-  </si>
-  <si>
-    <t>NNCRI</t>
-  </si>
-  <si>
-    <t>Costa Rica</t>
-  </si>
-  <si>
-    <t>NNSLV</t>
-  </si>
-  <si>
-    <t>El Salvador</t>
-  </si>
-  <si>
-    <t>NNGTM</t>
-  </si>
-  <si>
-    <t>Guatemala</t>
-  </si>
-  <si>
-    <t>NNHND</t>
-  </si>
-  <si>
-    <t>Honduras</t>
-  </si>
-  <si>
-    <t>NNMEX</t>
-  </si>
-  <si>
-    <t>México</t>
-  </si>
-  <si>
-    <t>NNNIC</t>
-  </si>
-  <si>
-    <t>Nicaragua</t>
-  </si>
-  <si>
-    <t>NNPAN</t>
-  </si>
-  <si>
-    <t>Panamá</t>
-  </si>
-  <si>
-    <t>NNARG</t>
-  </si>
-  <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>NNBOL</t>
-  </si>
-  <si>
-    <t>Bolivia</t>
-  </si>
-  <si>
-    <t>NNBRA</t>
-  </si>
-  <si>
-    <t>Brasil</t>
-  </si>
-  <si>
-    <t>NNCOL</t>
-  </si>
-  <si>
-    <t>Colombia</t>
-  </si>
-  <si>
-    <t>NNECU</t>
-  </si>
-  <si>
-    <t>Ecuador</t>
-  </si>
-  <si>
-    <t>NNGUY</t>
-  </si>
-  <si>
-    <t>Guyana</t>
-  </si>
-  <si>
-    <t>NNPRY</t>
-  </si>
-  <si>
-    <t>Paraguay</t>
-  </si>
-  <si>
-    <t>NNPER</t>
-  </si>
-  <si>
-    <t>Perú</t>
-  </si>
-  <si>
-    <t>NNSUR</t>
-  </si>
-  <si>
-    <t>Surinam</t>
-  </si>
-  <si>
-    <t>NNURY</t>
-  </si>
-  <si>
-    <t>Uruguay</t>
-  </si>
-  <si>
-    <t>NNVEN</t>
-  </si>
-  <si>
-    <t>Venezuela</t>
-  </si>
-  <si>
-    <t>NNCHL</t>
   </si>
   <si>
     <t>NNATG</t>
@@ -467,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -569,74 +566,66 @@
       <c r="A12" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="B12" t="s" s="2">
-        <v>23</v>
-      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="B15" t="s" s="2">
-        <v>27</v>
-      </c>
+      <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="B20" t="s" s="2">
-        <v>33</v>
-      </c>
+      <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s" s="2">
         <v>34</v>
-      </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s" s="2">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -654,411 +643,411 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s" s="1">
         <v>37</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="D1" t="s" s="1">
         <v>38</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>40</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s" s="2">
         <v>41</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>43</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s" s="2">
         <v>81</v>
-      </c>
-      <c r="C22" t="s" s="2">
-        <v>82</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s" s="2">
         <v>83</v>
-      </c>
-      <c r="C23" t="s" s="2">
-        <v>84</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="C24" t="s" s="2">
         <v>85</v>
-      </c>
-      <c r="C24" t="s" s="2">
-        <v>86</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s" s="2">
         <v>87</v>
-      </c>
-      <c r="C25" t="s" s="2">
-        <v>88</v>
       </c>
       <c r="D25" s="2"/>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="C26" t="s" s="2">
         <v>89</v>
-      </c>
-      <c r="C26" t="s" s="2">
-        <v>90</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="C27" t="s" s="2">
         <v>91</v>
-      </c>
-      <c r="C27" t="s" s="2">
-        <v>92</v>
       </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="C28" t="s" s="2">
         <v>93</v>
-      </c>
-      <c r="C28" t="s" s="2">
-        <v>94</v>
       </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="C29" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="C29" t="s" s="2">
-        <v>96</v>
       </c>
       <c r="D29" s="2"/>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s" s="2">
         <v>97</v>
-      </c>
-      <c r="C30" t="s" s="2">
-        <v>98</v>
       </c>
       <c r="D30" s="2"/>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="C31" t="s" s="2">
-        <v>100</v>
       </c>
       <c r="D31" s="2"/>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="C32" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="C32" t="s" s="2">
-        <v>102</v>
       </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="C33" t="s" s="2">
         <v>103</v>
-      </c>
-      <c r="C33" t="s" s="2">
-        <v>104</v>
       </c>
       <c r="D33" s="2"/>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="C34" t="s" s="2">
         <v>105</v>
-      </c>
-      <c r="C34" t="s" s="2">
-        <v>106</v>
       </c>
       <c r="D34" s="2"/>
     </row>

</xml_diff>